<commit_message>
Retta en feil i dataen
</commit_message>
<xml_diff>
--- a/Python code/Charpytest_resultater.xlsx
+++ b/Python code/Charpytest_resultater.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin-PC\Bilder\GitHub\TMT4171_mattek_Lab4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Robin-PC\Bilder\GitHub\TMT4171_mattek_Lab4\Python code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E03F65A-FBDD-439D-9D96-65B72FBE843A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D622CE7-48DC-42CB-A6D2-6E14688EBFD3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{3A66F279-13BF-4D9F-A326-7AC315BE7478}"/>
   </bookViews>
@@ -452,7 +452,7 @@
   <dimension ref="A1:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -594,7 +594,7 @@
         <v>21</v>
       </c>
       <c r="E10">
-        <v>102</v>
+        <v>71</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>